<commit_message>
add contact email and fix lat-vs-lng
</commit_message>
<xml_diff>
--- a/resources/excel/20241024 CodeWeek activities NOVEMBER CoderDojo Belgium.xlsx
+++ b/resources/excel/20241024 CodeWeek activities NOVEMBER CoderDojo Belgium.xlsx
@@ -55,10 +55,10 @@
     <t>Contact email</t>
   </si>
   <si>
+    <t>Latitude</t>
+  </si>
+  <si>
     <t>Longitude</t>
-  </si>
-  <si>
-    <t>Latitude</t>
   </si>
   <si>
     <t>Image path</t>
@@ -98,7 +98,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="10"/>
+        <color indexed="11"/>
         <rFont val="Arial"/>
       </rPr>
       <t>https://www.coderdojobelgium.be</t>
@@ -298,16 +298,22 @@
     <font>
       <u val="single"/>
       <sz val="10"/>
-      <color indexed="10"/>
+      <color indexed="11"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -320,16 +326,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -346,22 +352,22 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="60" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -381,6 +387,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff0000ff"/>
     </indexedColors>
@@ -581,12 +588,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -618,10 +625,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -860,12 +867,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1169,10 +1176,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">

</xml_diff>